<commit_message>
saved a latest copy
</commit_message>
<xml_diff>
--- a/Documentation/KEC_Project_Management.xlsx
+++ b/Documentation/KEC_Project_Management.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Project Management" sheetId="1" r:id="rId1"/>
@@ -385,9 +385,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -395,6 +392,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -468,11 +468,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A2:B9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A2:B9" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A2:B9"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Page " dataDxfId="3"/>
-    <tableColumn id="2" name="Task" dataDxfId="2"/>
+    <tableColumn id="1" name="Page " dataDxfId="1"/>
+    <tableColumn id="2" name="Task" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -767,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -784,8 +784,8 @@
       <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -796,8 +796,8 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -948,8 +948,8 @@
       <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -987,7 +987,7 @@
       <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C4" t="s">
@@ -1039,7 +1039,7 @@
       <c r="A6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C6" t="s">
@@ -1091,7 +1091,7 @@
       <c r="A8" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C8" t="s">
@@ -1126,7 +1126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1137,66 +1137,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added some more to-do tasks
</commit_message>
<xml_diff>
--- a/Documentation/KEC_Project_Management.xlsx
+++ b/Documentation/KEC_Project_Management.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Project Management" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="F8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Need actua links for twitter and linkedin</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
   <si>
     <t>Project Type</t>
   </si>
@@ -212,9 +246,6 @@
     <t>Menu Addition</t>
   </si>
   <si>
-    <t>Add new Menu : FAQ's and Add all FAQ's from http://laparoscopyexpert.com/faq_for_patient.html</t>
-  </si>
-  <si>
     <t>Page/Change Area</t>
   </si>
   <si>
@@ -254,9 +285,6 @@
     <t>FAQ </t>
   </si>
   <si>
-    <t>In Progress.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Footer </t>
   </si>
   <si>
@@ -267,13 +295,80 @@
   </si>
   <si>
     <t>Contact US</t>
+  </si>
+  <si>
+    <t>Add new Menu : FAQ's and Add all FAQ's from http://laparoscopyexpert.com/faq_for_patient.html (Ameer: As per the Testimonials page)</t>
+  </si>
+  <si>
+    <t>Mubasshir and Veena</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Completion Date</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>Veena</t>
+  </si>
+  <si>
+    <t>1. Add FAQ's from : http://laparoscopyexpert.com/faq_for_patient.html 
+2. Remove "For patients" &amp; show directly under FAQ's (Ameer)</t>
+  </si>
+  <si>
+    <t>All Pages</t>
+  </si>
+  <si>
+    <t>Color of "Home / Meet the Doctor" should get changed to "Home (dark pink used in app)/ Meet the Doctor" (Ameer)</t>
+  </si>
+  <si>
+    <t>Could see significant blank space on top of actual page design of all pages. For e.g. just see above "Home / About Us" text on about us page. (Ameer)</t>
+  </si>
+  <si>
+    <t>Change background color of "Read More" or any other relevant component from blue to Dark Pink &amp; &amp; use label color as white for same. (Ameer)</t>
+  </si>
+  <si>
+    <t>Minimize the white space in top bar (Ameer)</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Defect</t>
+  </si>
+  <si>
+    <t>On Services main page link for "Infertility" is missing in page. As of now only two links are provided. (Ameer)</t>
+  </si>
+  <si>
+    <t>On Services drop down if I select "Infertility" it doesn't move to that page. It should navigate to overview page. (Ameer)</t>
+  </si>
+  <si>
+    <t>Top Navigation - Services</t>
+  </si>
+  <si>
+    <t>Breadcrumb</t>
+  </si>
+  <si>
+    <t>On selection of any navigation item it starts with "Home / Meet the Doctor". Rather it should start with actual navigation item for e.g "About Us / Meet the Doctor". (Ameer)</t>
+  </si>
+  <si>
+    <t>Integration of Actual KEC Images</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +423,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -381,7 +489,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
@@ -397,13 +505,28 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -468,11 +591,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A2:B9" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A2:B9"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Page " dataDxfId="1"/>
-    <tableColumn id="2" name="Task" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A2:F17" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:F17"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Page " dataDxfId="5"/>
+    <tableColumn id="2" name="Task" dataDxfId="4"/>
+    <tableColumn id="3" name="Category" dataDxfId="3"/>
+    <tableColumn id="4" name="Resource" dataDxfId="2"/>
+    <tableColumn id="5" name="Completion Date" dataDxfId="1"/>
+    <tableColumn id="6" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -767,7 +894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -830,7 +957,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -924,7 +1051,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +1059,7 @@
     <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
@@ -959,7 +1086,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -1087,18 +1214,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
         <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="E8" s="1">
         <v>42401</v>
@@ -1106,8 +1233,11 @@
       <c r="F8" s="1">
         <v>42403</v>
       </c>
+      <c r="H8" s="1">
+        <v>42405</v>
+      </c>
       <c r="I8" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1123,87 +1253,322 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.5703125" customWidth="1"/>
     <col min="2" max="2" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="7">
+        <v>42405</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="C8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>59</v>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="7">
+        <v>42405</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="7">
+        <v>42405</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="7">
+        <v>42405</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="7">
+        <v>42405</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="7">
+        <v>42405</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="7">
+        <v>42405</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="7">
+        <v>42405</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>